<commit_message>
Updated data with 2 studies
Added two studies found in https://link.springer.com/article/10.1186/s13102-021-00335-8#ref-CR37
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90399512-DF82-45D9-9832-8F8902FA469E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE55DC23-1280-40D7-BD20-988A560EC8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_characteristics" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4413" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4432" uniqueCount="1279">
   <si>
     <t>study_id</t>
   </si>
@@ -3950,6 +3950,24 @@
   </si>
   <si>
     <t>week-to-week % change, accumulated exposure time</t>
+  </si>
+  <si>
+    <t>Hartwig</t>
+  </si>
+  <si>
+    <t>Training and match volume and injury in adolescents playing multiple contact team sports: A prospective cohort study</t>
+  </si>
+  <si>
+    <t>Incidence and prevalence of lumbar stress fracture in English County Cricket fast bowlers, association with bowling workload and seasonal variation</t>
+  </si>
+  <si>
+    <t>Alway</t>
+  </si>
+  <si>
+    <t>Is risk of fast bowling injury in cricketers greatest in those who bowl most? A cohort of young English fast bowlers</t>
+  </si>
+  <si>
+    <t>Gregory</t>
   </si>
 </sst>
 </file>
@@ -4515,13 +4533,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU154"/>
+  <dimension ref="A1:AU157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G135" sqref="G135"/>
+      <selection pane="bottomRight" activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17937,6 +17955,123 @@
         <v>48</v>
       </c>
       <c r="AK154" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="155" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>158</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C155">
+        <v>2019</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1274</v>
+      </c>
+      <c r="G155" t="s">
+        <v>634</v>
+      </c>
+      <c r="H155">
+        <v>103</v>
+      </c>
+      <c r="I155">
+        <v>103</v>
+      </c>
+      <c r="U155">
+        <v>83</v>
+      </c>
+      <c r="V155">
+        <v>83</v>
+      </c>
+      <c r="Z155" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF155" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK155" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL155" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="156" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>159</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C156">
+        <v>2019</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1275</v>
+      </c>
+      <c r="G156" t="s">
+        <v>33</v>
+      </c>
+      <c r="H156">
+        <v>368</v>
+      </c>
+      <c r="I156">
+        <v>368</v>
+      </c>
+      <c r="U156">
+        <v>57</v>
+      </c>
+      <c r="V156">
+        <v>57</v>
+      </c>
+      <c r="Z156" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF156" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK156" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="157" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>160</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C157">
+        <v>2004</v>
+      </c>
+      <c r="D157" t="s">
+        <v>1277</v>
+      </c>
+      <c r="G157" t="s">
+        <v>33</v>
+      </c>
+      <c r="H157">
+        <v>70</v>
+      </c>
+      <c r="I157">
+        <v>70</v>
+      </c>
+      <c r="U157">
+        <v>23</v>
+      </c>
+      <c r="V157">
+        <v>23</v>
+      </c>
+      <c r="Z157" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF157" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK157" t="s">
         <v>48</v>
       </c>
     </row>
@@ -18064,13 +18199,13 @@
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155:AK439</xm:sqref>
+          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK158:AK439</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD855EAF-C81E-44C4-996E-D61F7541B9CE}">
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\arkiv\2021-06-08\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AL150:AL437 AK154</xm:sqref>
+          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AL150:AL437 AK156:AK157</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added one more study to data
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE55DC23-1280-40D7-BD20-988A560EC8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8463F793-D9A5-410A-B020-6DCD6BB5459F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_characteristics" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4432" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4440" uniqueCount="1282">
   <si>
     <t>study_id</t>
   </si>
@@ -3968,6 +3968,15 @@
   </si>
   <si>
     <t>Gregory</t>
+  </si>
+  <si>
+    <t>Chronic Workload, Subjective Arm Health, and Throwing Injury in High School Baseball Players: 3-Year Retrospective Pilot Study</t>
+  </si>
+  <si>
+    <t>throwing-related injury</t>
+  </si>
+  <si>
+    <t>28-day rolling average chronic load</t>
   </si>
 </sst>
 </file>
@@ -4533,13 +4542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU157"/>
+  <dimension ref="A1:AU158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AD135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G156" sqref="G156"/>
+      <selection pane="bottomRight" activeCell="AK158" sqref="AK158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18075,6 +18084,50 @@
         <v>48</v>
       </c>
     </row>
+    <row r="158" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>161</v>
+      </c>
+      <c r="B158" t="s">
+        <v>367</v>
+      </c>
+      <c r="C158">
+        <v>2021</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G158" t="s">
+        <v>36</v>
+      </c>
+      <c r="H158">
+        <v>49</v>
+      </c>
+      <c r="I158">
+        <v>49</v>
+      </c>
+      <c r="S158" s="24" t="s">
+        <v>1280</v>
+      </c>
+      <c r="U158">
+        <v>24</v>
+      </c>
+      <c r="V158">
+        <v>20</v>
+      </c>
+      <c r="Z158" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA158" t="s">
+        <v>1281</v>
+      </c>
+      <c r="AF158" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK158" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU99">
     <sortCondition ref="A1"/>
@@ -18084,7 +18137,7 @@
       <formula1>0</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA109:AA119 T2:T47 Z19:Z47 AB30:AB46 W2:W47 AL2:AL46 AG2:AG46 AL131 AE2:AE46 AB2:AB28 E2:G47 AA122 AR28 AR31:AR45 AR2:AR26 Y2:Y47 Z2:Z17 L2:L47 AA125:AA126 AA128 S119 T121 S123:S124 AF2:AF47 S127:S128 T132 AL137:AL138 T134:T136 AK2:AK47 AL149 AA155:AA467 S131:S467 T138:T467" xr:uid="{6E4000BB-A1AB-4705-8E21-48EABE9449AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA109:AA119 T2:T47 Z19:Z47 AB30:AB46 W2:W47 AL2:AL46 AG2:AG46 AL131 AE2:AE46 AB2:AB28 E2:G47 AA122 AR28 AR31:AR45 AR2:AR26 Y2:Y47 Z2:Z17 L2:L47 AA125:AA126 AA128 S119 T121 S123:S124 AF2:AF47 S127:S128 T132 AL137:AL138 T134:T136 AK2:AK47 AL149 S159:S467 T138:T467 S131:S157 AA159:AA467" xr:uid="{6E4000BB-A1AB-4705-8E21-48EABE9449AE}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H29:I65 H28 I66 H67:I118 H6:I27 J9:J10 J12 J14:J88 J90:J118 K48:K118 H124:I125 H119:J123 J124 U6:U126 V6:V149 V151:V439 U129:U439 H126:J439 AH2:AH467 K120:K467" xr:uid="{60D466E1-2DC3-4BFC-8071-EF77CA5FF633}">
@@ -18199,13 +18252,13 @@
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK158:AK439</xm:sqref>
+          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK159:AK439</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD855EAF-C81E-44C4-996E-D61F7541B9CE}">
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\arkiv\2021-06-08\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AL150:AL437 AK156:AK157</xm:sqref>
+          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AL150:AL437 AK156:AK158</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added another study, finally some ice hockey
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8463F793-D9A5-410A-B020-6DCD6BB5459F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123C30D3-07EB-4D78-84D2-44998FC0B447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_characteristics" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4440" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4446" uniqueCount="1285">
   <si>
     <t>study_id</t>
   </si>
@@ -3977,6 +3977,15 @@
   </si>
   <si>
     <t>28-day rolling average chronic load</t>
+  </si>
+  <si>
+    <t>Effects of training load and non-training stress on injury risk in collegiate ice hockey players</t>
+  </si>
+  <si>
+    <t>Mustapich</t>
+  </si>
+  <si>
+    <t>Ice hockey</t>
   </si>
 </sst>
 </file>
@@ -4542,13 +4551,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU158"/>
+  <dimension ref="A1:AU159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AD135" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M141" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK158" sqref="AK158"/>
+      <selection pane="bottomRight" activeCell="T159" sqref="T159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18128,6 +18137,29 @@
         <v>48</v>
       </c>
     </row>
+    <row r="159" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>162</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C159">
+        <v>2021</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1282</v>
+      </c>
+      <c r="G159" t="s">
+        <v>1284</v>
+      </c>
+      <c r="Z159" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF159" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU99">
     <sortCondition ref="A1"/>
@@ -18154,15 +18186,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="18">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{033943A1-CF9A-42A9-8B86-C1FB4B53C2EF}">
           <x14:formula1>
-            <xm:f>codebook!$C$37:$C$44</xm:f>
+            <xm:f>codebook!$C$38:$C$45</xm:f>
           </x14:formula1>
-          <xm:sqref>AB29 AB47:AB93 AB102:AB104 AB106:AB108 AB100 AB129:AB467</xm:sqref>
+          <xm:sqref>AB29 AB129:AB467 AB100 AB106:AB108 AB102:AB104 AB47:AB93</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F238D84F-257C-4E80-BC93-470E9165C497}">
           <x14:formula1>
-            <xm:f>codebook!$C$68:$C$69</xm:f>
+            <xm:f>codebook!$C$69:$C$70</xm:f>
           </x14:formula1>
-          <xm:sqref>AR29:AR30 AR102:AR104 AR27 AR46:AR93 AR106:AR108 AR100 AR129:AR467</xm:sqref>
+          <xm:sqref>AR29:AR30 AR129:AR467 AR100 AR106:AR108 AR46:AR93 AR27 AR102:AR104</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7962E7F5-5013-458E-80A5-C8B1D0CB9F3D}">
           <x14:formula1>
@@ -18184,57 +18216,57 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DAA2A116-C546-467D-B789-84B30BBF42B8}">
           <x14:formula1>
-            <xm:f>codebook!$C$70:$C$75</xm:f>
+            <xm:f>codebook!$C$71:$C$76</xm:f>
           </x14:formula1>
           <xm:sqref>W48:W65 W75:W76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56F6F299-23C3-44BD-9B2C-75916FC9C121}">
           <x14:formula1>
-            <xm:f>codebook!$C$81:$C$83</xm:f>
+            <xm:f>codebook!$C$82:$C$84</xm:f>
           </x14:formula1>
-          <xm:sqref>Y48:Y93 Y100 Y106:Y108 Y102:Y104 Y129:Y467</xm:sqref>
+          <xm:sqref>Y48:Y93 Y129:Y467 Y102:Y104 Y106:Y108 Y100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{965DCBF5-E627-4FAF-B5EA-6026C44EBFF2}">
           <x14:formula1>
-            <xm:f>codebook!$C$33:$C$36</xm:f>
+            <xm:f>codebook!$C$34:$C$37</xm:f>
           </x14:formula1>
-          <xm:sqref>Z18 Z48:Z93 Z102:Z104 Z106:Z108 Z100 Z129:Z467</xm:sqref>
+          <xm:sqref>Z18 Z129:Z467 Z100 Z106:Z108 Z102:Z104 Z48:Z93</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{76937EA2-83C8-482C-89B8-C27ED8037D80}">
           <x14:formula1>
-            <xm:f>codebook!$C$29:$C$30</xm:f>
+            <xm:f>codebook!$C$30:$C$31</xm:f>
           </x14:formula1>
-          <xm:sqref>AE47:AE93 AE102:AE104 AE106:AE108 AE100 AE129:AE467</xm:sqref>
+          <xm:sqref>AE47:AE93 AE129:AE467 AE100 AE106:AE108 AE102:AE104</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0C43AC12-0D7E-4339-B4A5-387DE632A39A}">
           <x14:formula1>
-            <xm:f>codebook!$C$31:$C$32</xm:f>
+            <xm:f>codebook!$C$32:$C$33</xm:f>
           </x14:formula1>
-          <xm:sqref>AF48:AF93 AF102:AF104 AF106:AF108 AF100 AF129:AF467</xm:sqref>
+          <xm:sqref>AF48:AF93 AF129:AF467 AF100 AF106:AF108 AF102:AF104</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E8F7E910-9B70-48C5-85EB-0D70379483B7}">
           <x14:formula1>
-            <xm:f>codebook!$C$45:$C$56</xm:f>
+            <xm:f>codebook!$C$46:$C$57</xm:f>
           </x14:formula1>
-          <xm:sqref>AG47:AG93 AG100 AG106:AG108 AG102:AG104 AG129:AG467</xm:sqref>
+          <xm:sqref>AG47:AG93 AG129:AG467 AG102:AG104 AG106:AG108 AG100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{510E9D53-4274-4B09-BB41-5D64F2B99D2C}">
           <x14:formula1>
-            <xm:f>codebook!$C$84:$C$86</xm:f>
+            <xm:f>codebook!$C$85:$C$87</xm:f>
           </x14:formula1>
-          <xm:sqref>T102:T104 T132 T129:T130 T100 T106:T108 T48:T93 T134:T467</xm:sqref>
+          <xm:sqref>T102:T104 T134:T467 T48:T93 T106:T108 T100 T129:T130 T132</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{900463C5-0ADF-47C5-9EE5-FFD02FB58F86}">
           <x14:formula1>
-            <xm:f>codebook!$C$8:$C$25</xm:f>
+            <xm:f>codebook!$C$8:$C$26</xm:f>
           </x14:formula1>
-          <xm:sqref>G66:G93 G102:G104 G106:G108 G100 G129:G470</xm:sqref>
+          <xm:sqref>G66:G93 G129:G470 G100 G106:G108 G102:G104</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{30C25733-E64C-466F-9988-EBA8C30F2241}">
           <x14:formula1>
-            <xm:f>codebook!$C$70:$C$80</xm:f>
+            <xm:f>codebook!$C$71:$C$81</xm:f>
           </x14:formula1>
-          <xm:sqref>W66:W74 W98 W102:W108 W77:W93 W130:W471</xm:sqref>
+          <xm:sqref>W66:W74 W130:W471 W77:W93 W102:W108 W98</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1404BC5-4FF5-4C04-B486-DE592A3F3DB4}">
           <x14:formula1>
@@ -18271,7 +18303,7 @@
   <dimension ref="A1:F283"/>
   <sheetViews>
     <sheetView topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="C283" sqref="C283"/>
+      <selection activeCell="C300" sqref="C300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21719,27 +21751,27 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8AC3997-9850-4D0F-BE39-23883909EC25}">
           <x14:formula1>
-            <xm:f>codebook!$C$87:$C$121</xm:f>
+            <xm:f>codebook!$C$88:$C$122</xm:f>
           </x14:formula1>
-          <xm:sqref>B100 B279:B626 B76 B22 B112:B219 B231:B248 C360:C626</xm:sqref>
+          <xm:sqref>B100 C360:C626 B231:B248 B112:B219 B22 B76 B279:B626</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FA48F9AD-477C-41FE-97D8-9AD05DED636F}">
           <x14:formula1>
-            <xm:f>codebook!$C$133:$C$134</xm:f>
+            <xm:f>codebook!$C$134:$C$135</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F173 F267:F273 F263 F261 F258 F278:F460 F231:F248 F175:F219</xm:sqref>
+          <xm:sqref>F2:F173 F175:F219 F231:F248 F278:F460 F258 F261 F263 F267:F273</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2460B3D9-2072-4464-9488-612B96EFB2E9}">
           <x14:formula1>
-            <xm:f>codebook!$C$124:$C$129</xm:f>
+            <xm:f>codebook!$C$125:$C$130</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C219 C278:C359 C231:C248</xm:sqref>
+          <xm:sqref>C2:C219 C231:C248 C278:C359</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{04A790D0-A615-4B6C-9BDC-FC8B8EE8C3AC}">
           <x14:formula1>
-            <xm:f>codebook!$C$175:$C$177</xm:f>
+            <xm:f>codebook!$C$176:$C$178</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E219 E278:E626 E231:E248</xm:sqref>
+          <xm:sqref>E2:E219 E231:E248 E278:E626</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B43BAAAC-1456-4172-9CF9-606CEA860D5F}">
           <x14:formula1>
@@ -22610,15 +22642,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2C06C4C4-7BE4-4595-B3FF-1B88F7AE9525}">
           <x14:formula1>
-            <xm:f>codebook!$C$147:$C$174</xm:f>
+            <xm:f>codebook!$C$148:$C$175</xm:f>
           </x14:formula1>
-          <xm:sqref>C24:C45 C62:C631 C47:C54</xm:sqref>
+          <xm:sqref>C24:C45 C47:C54 C62:C631</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BDAAE0E-9072-48C3-A217-6517A70E8E8C}">
           <x14:formula1>
-            <xm:f>codebook!$C$135:$C$146</xm:f>
+            <xm:f>codebook!$C$136:$C$147</xm:f>
           </x14:formula1>
-          <xm:sqref>B24:B45 B62:B631 B47:B54</xm:sqref>
+          <xm:sqref>B24:B45 B47:B54 B62:B631</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5407EE94-21A5-4331-A79D-6AFA5E8047EC}">
           <x14:formula1>
@@ -24466,10 +24498,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D57AF8F-1D16-4411-BBD5-963EC5A9A56B}">
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24621,7 +24653,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
@@ -24629,7 +24661,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -24637,7 +24669,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -24645,7 +24677,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>689</v>
@@ -24653,7 +24685,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>771</v>
@@ -24661,7 +24693,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
         <v>999</v>
@@ -24669,7 +24701,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>1229</v>
@@ -24677,1290 +24709,1298 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>1259</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>1</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>15</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>0</v>
       </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30">
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31">
         <v>1</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>0</v>
       </c>
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>1</v>
-      </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>27</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>1</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>208</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>709</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>408</v>
+        <v>709</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>443</v>
+        <v>408</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45">
         <v>99</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>24</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>2</v>
-      </c>
-      <c r="C46" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>216</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>672</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>1190</v>
+        <v>672</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57">
         <v>99</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>16</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>0</v>
       </c>
-      <c r="C57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <v>1</v>
-      </c>
       <c r="C58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>17</v>
-      </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60">
-        <v>2</v>
-      </c>
-      <c r="C60" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>277</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>702</v>
+        <v>277</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>1271</v>
+        <v>702</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68">
         <v>99</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>462</v>
       </c>
-      <c r="B68">
+      <c r="B69">
         <v>0</v>
       </c>
-      <c r="C68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69">
-        <v>1</v>
-      </c>
       <c r="C69" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>10</v>
-      </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71">
-        <v>2</v>
-      </c>
-      <c r="C71" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>469</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>107</v>
+        <v>469</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>658</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>635</v>
+        <v>658</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>918</v>
+        <v>635</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>1035</v>
+        <v>918</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B81">
         <v>11</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>11</v>
       </c>
-      <c r="B81">
+      <c r="B82">
         <v>1</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B82">
-        <v>2</v>
-      </c>
-      <c r="C82" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84">
         <v>3</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>19</v>
       </c>
-      <c r="B84">
+      <c r="B85">
         <v>1</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B85">
-        <v>2</v>
-      </c>
-      <c r="C85" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87">
         <v>3</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>68</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>1</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88">
-        <v>2</v>
-      </c>
-      <c r="C88" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>69</v>
+        <v>475</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>1157</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>578</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>72</v>
+        <v>578</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>377</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C102" t="s">
-        <v>376</v>
+        <v>79</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>17</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="C103" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>369</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>81</v>
+        <v>369</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>447</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>390</v>
+        <v>447</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>87</v>
+        <v>390</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>370</v>
+        <v>91</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>92</v>
+        <v>371</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>1156</v>
+        <v>92</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>375</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B123">
+        <v>36</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B124">
         <v>37</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C124" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>729</v>
       </c>
-      <c r="B124">
+      <c r="B125">
         <v>0</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C125" s="3" t="s">
         <v>730</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B125">
-        <v>1</v>
-      </c>
-      <c r="C125" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B126">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B127">
-        <v>3</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>731</v>
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B130">
         <v>5</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="C130" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B130">
+      <c r="B131">
         <v>1</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>364</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B131">
-        <v>2</v>
-      </c>
-      <c r="C131" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B133">
         <v>3</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>593</v>
       </c>
-      <c r="B133">
+      <c r="B134">
         <v>1</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B135">
         <v>2</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C135" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>411</v>
       </c>
-      <c r="B135">
+      <c r="B136">
         <v>1</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136">
-        <v>2</v>
-      </c>
-      <c r="C136" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C137" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C138" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>582</v>
+        <v>413</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>417</v>
+        <v>582</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C143" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C144" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C145" t="s">
-        <v>695</v>
+        <v>415</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146">
+        <v>11</v>
+      </c>
+      <c r="C146" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B147">
         <v>12</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C147" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>343</v>
       </c>
-      <c r="B147">
+      <c r="B148">
         <v>1</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C148" t="s">
         <v>344</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B148">
-        <v>2</v>
-      </c>
-      <c r="C148" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C149" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C150" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>380</v>
+        <v>348</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B152">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C152" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>349</v>
+        <v>420</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C154" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C155" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C156" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B157">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C157" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C158" t="s">
-        <v>421</v>
+        <v>351</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C159" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B160">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C160" t="s">
-        <v>513</v>
+        <v>422</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C161" t="s">
-        <v>581</v>
+        <v>513</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C162" t="s">
-        <v>361</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C163" t="s">
-        <v>590</v>
+        <v>361</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C164" t="s">
-        <v>352</v>
+        <v>590</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C165" t="s">
-        <v>692</v>
+        <v>352</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C166" t="s">
-        <v>353</v>
+        <v>692</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C167" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C168" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C169" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C170" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C171" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C172" t="s">
-        <v>696</v>
+        <v>358</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C173" t="s">
-        <v>359</v>
+        <v>696</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B174">
+        <v>27</v>
+      </c>
+      <c r="C174" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B175">
         <v>28</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C175" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>401</v>
       </c>
-      <c r="B175">
+      <c r="B176">
         <v>1</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B176">
-        <v>2</v>
-      </c>
-      <c r="C176" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177">
+        <v>2</v>
+      </c>
+      <c r="C177" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178">
         <v>99</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C178" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added study published today
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123C30D3-07EB-4D78-84D2-44998FC0B447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383020A9-B20B-4AAE-ADAD-4ADDD41C61AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4446" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4456" uniqueCount="1287">
   <si>
     <t>study_id</t>
   </si>
@@ -3986,6 +3986,12 @@
   </si>
   <si>
     <t>Ice hockey</t>
+  </si>
+  <si>
+    <t>Nordstrøm</t>
+  </si>
+  <si>
+    <t>Association of Training and Game Loads to Injury Risk in Junior Male Elite Ice Hockey Players: A Prospective Cohort Study</t>
   </si>
 </sst>
 </file>
@@ -4551,13 +4557,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU159"/>
+  <dimension ref="A1:AU160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M141" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T159" sqref="T159"/>
+      <selection pane="bottomRight" activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18158,6 +18164,56 @@
       </c>
       <c r="AF159" t="s">
         <v>49</v>
+      </c>
+      <c r="AK159" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="160" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>163</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C160">
+        <v>2022</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E160" t="s">
+        <v>28</v>
+      </c>
+      <c r="F160" t="s">
+        <v>210</v>
+      </c>
+      <c r="G160" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H160">
+        <v>159</v>
+      </c>
+      <c r="I160">
+        <v>159</v>
+      </c>
+      <c r="U160">
+        <v>133</v>
+      </c>
+      <c r="V160">
+        <v>133</v>
+      </c>
+      <c r="Z160" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF160" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK160" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL160" t="s">
+        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -18284,13 +18340,13 @@
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK159:AK439</xm:sqref>
+          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK160:AK439</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD855EAF-C81E-44C4-996E-D61F7541B9CE}">
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\arkiv\2021-06-08\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AL150:AL437 AK156:AK158</xm:sqref>
+          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AK156:AK159 AL150:AL437</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added more articles published in November 2022
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383020A9-B20B-4AAE-ADAD-4ADDD41C61AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E15E8A6-BCAC-4769-B814-6E49CFACEF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4456" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4466" uniqueCount="1291">
   <si>
     <t>study_id</t>
   </si>
@@ -3992,6 +3992,18 @@
   </si>
   <si>
     <t>Association of Training and Game Loads to Injury Risk in Junior Male Elite Ice Hockey Players: A Prospective Cohort Study</t>
+  </si>
+  <si>
+    <t>Team's Average Acute:Chronic Workload Ratio Correlates with Injury Risk in NCAA Men's Soccer Team</t>
+  </si>
+  <si>
+    <t>Bakal</t>
+  </si>
+  <si>
+    <t>Noncontact Injury Distribution and Relationship With Preseason Training Load and Nonmodifiable Risk Factors in Rugby Union Players Across Multiple Seasons</t>
+  </si>
+  <si>
+    <t>Evans</t>
   </si>
 </sst>
 </file>
@@ -4557,13 +4569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU160"/>
+  <dimension ref="A1:AU162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AA143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A160" sqref="A160"/>
+      <selection pane="bottomRight" activeCell="AK162" sqref="AK162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18214,6 +18226,52 @@
       </c>
       <c r="AL160" t="s">
         <v>702</v>
+      </c>
+    </row>
+    <row r="161" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>164</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C161">
+        <v>2022</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1287</v>
+      </c>
+      <c r="G161" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z161" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF161" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="162" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>165</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C162">
+        <v>2022</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1289</v>
+      </c>
+      <c r="G162" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z162" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF162" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with December studies and a missed January study
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E15E8A6-BCAC-4769-B814-6E49CFACEF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC17C44-2FEF-42A4-BD77-6BF1F287C514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
+    <workbookView xWindow="4335" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_characteristics" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4466" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4481" uniqueCount="1296">
   <si>
     <t>study_id</t>
   </si>
@@ -4004,6 +4004,21 @@
   </si>
   <si>
     <t>Evans</t>
+  </si>
+  <si>
+    <t>Sonesson</t>
+  </si>
+  <si>
+    <t>Risk factors for injury and illness in youth floorball players – A prospective cohort study</t>
+  </si>
+  <si>
+    <t>Floorball</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Analysis of the injuries and workload evolution using the RPE and s-RPE method in basketball</t>
   </si>
 </sst>
 </file>
@@ -4569,13 +4584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU162"/>
+  <dimension ref="A1:AU164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AA143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AD145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK162" sqref="AK162"/>
+      <selection pane="bottomRight" activeCell="AD155" sqref="AD155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18228,7 +18243,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="161" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>164</v>
       </c>
@@ -18251,7 +18266,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="162" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>165</v>
       </c>
@@ -18272,6 +18287,76 @@
       </c>
       <c r="AF162" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="163" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>166</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C163">
+        <v>2022</v>
+      </c>
+      <c r="D163" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E163" t="s">
+        <v>28</v>
+      </c>
+      <c r="F163" t="s">
+        <v>210</v>
+      </c>
+      <c r="G163" t="s">
+        <v>1293</v>
+      </c>
+      <c r="Z163" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF163" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK163" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="164" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>167</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C164">
+        <v>2022</v>
+      </c>
+      <c r="D164" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G164" t="s">
+        <v>39</v>
+      </c>
+      <c r="H164">
+        <v>9</v>
+      </c>
+      <c r="I164">
+        <v>9</v>
+      </c>
+      <c r="U164">
+        <v>14</v>
+      </c>
+      <c r="V164">
+        <v>14</v>
+      </c>
+      <c r="Z164" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF164" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK164" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -18300,15 +18385,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="18">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{033943A1-CF9A-42A9-8B86-C1FB4B53C2EF}">
           <x14:formula1>
-            <xm:f>codebook!$C$38:$C$45</xm:f>
+            <xm:f>codebook!$C$39:$C$46</xm:f>
           </x14:formula1>
-          <xm:sqref>AB29 AB129:AB467 AB100 AB106:AB108 AB102:AB104 AB47:AB93</xm:sqref>
+          <xm:sqref>AB29 AB47:AB93 AB102:AB104 AB106:AB108 AB100 AB129:AB467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F238D84F-257C-4E80-BC93-470E9165C497}">
           <x14:formula1>
-            <xm:f>codebook!$C$69:$C$70</xm:f>
+            <xm:f>codebook!$C$70:$C$71</xm:f>
           </x14:formula1>
-          <xm:sqref>AR29:AR30 AR129:AR467 AR100 AR106:AR108 AR46:AR93 AR27 AR102:AR104</xm:sqref>
+          <xm:sqref>AR29:AR30 AR102:AR104 AR27 AR46:AR93 AR106:AR108 AR100 AR129:AR467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7962E7F5-5013-458E-80A5-C8B1D0CB9F3D}">
           <x14:formula1>
@@ -18330,57 +18415,57 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DAA2A116-C546-467D-B789-84B30BBF42B8}">
           <x14:formula1>
-            <xm:f>codebook!$C$71:$C$76</xm:f>
+            <xm:f>codebook!$C$72:$C$77</xm:f>
           </x14:formula1>
           <xm:sqref>W48:W65 W75:W76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56F6F299-23C3-44BD-9B2C-75916FC9C121}">
           <x14:formula1>
-            <xm:f>codebook!$C$82:$C$84</xm:f>
+            <xm:f>codebook!$C$83:$C$85</xm:f>
           </x14:formula1>
-          <xm:sqref>Y48:Y93 Y129:Y467 Y102:Y104 Y106:Y108 Y100</xm:sqref>
+          <xm:sqref>Y48:Y93 Y100 Y106:Y108 Y102:Y104 Y129:Y467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{965DCBF5-E627-4FAF-B5EA-6026C44EBFF2}">
           <x14:formula1>
-            <xm:f>codebook!$C$34:$C$37</xm:f>
+            <xm:f>codebook!$C$35:$C$38</xm:f>
           </x14:formula1>
-          <xm:sqref>Z18 Z129:Z467 Z100 Z106:Z108 Z102:Z104 Z48:Z93</xm:sqref>
+          <xm:sqref>Z18 Z48:Z93 Z102:Z104 Z106:Z108 Z100 Z129:Z467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{76937EA2-83C8-482C-89B8-C27ED8037D80}">
           <x14:formula1>
-            <xm:f>codebook!$C$30:$C$31</xm:f>
+            <xm:f>codebook!$C$31:$C$32</xm:f>
           </x14:formula1>
-          <xm:sqref>AE47:AE93 AE129:AE467 AE100 AE106:AE108 AE102:AE104</xm:sqref>
+          <xm:sqref>AE47:AE93 AE102:AE104 AE106:AE108 AE100 AE129:AE467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0C43AC12-0D7E-4339-B4A5-387DE632A39A}">
           <x14:formula1>
-            <xm:f>codebook!$C$32:$C$33</xm:f>
+            <xm:f>codebook!$C$33:$C$34</xm:f>
           </x14:formula1>
-          <xm:sqref>AF48:AF93 AF129:AF467 AF100 AF106:AF108 AF102:AF104</xm:sqref>
+          <xm:sqref>AF48:AF93 AF102:AF104 AF106:AF108 AF100 AF129:AF467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E8F7E910-9B70-48C5-85EB-0D70379483B7}">
           <x14:formula1>
-            <xm:f>codebook!$C$46:$C$57</xm:f>
+            <xm:f>codebook!$C$47:$C$58</xm:f>
           </x14:formula1>
-          <xm:sqref>AG47:AG93 AG129:AG467 AG102:AG104 AG106:AG108 AG100</xm:sqref>
+          <xm:sqref>AG47:AG93 AG100 AG106:AG108 AG102:AG104 AG129:AG467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{510E9D53-4274-4B09-BB41-5D64F2B99D2C}">
           <x14:formula1>
-            <xm:f>codebook!$C$85:$C$87</xm:f>
+            <xm:f>codebook!$C$86:$C$88</xm:f>
           </x14:formula1>
-          <xm:sqref>T102:T104 T134:T467 T48:T93 T106:T108 T100 T129:T130 T132</xm:sqref>
+          <xm:sqref>T102:T104 T132 T129:T130 T100 T106:T108 T48:T93 T134:T467</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{900463C5-0ADF-47C5-9EE5-FFD02FB58F86}">
           <x14:formula1>
-            <xm:f>codebook!$C$8:$C$26</xm:f>
+            <xm:f>codebook!$C$8:$C$27</xm:f>
           </x14:formula1>
-          <xm:sqref>G66:G93 G129:G470 G100 G106:G108 G102:G104</xm:sqref>
+          <xm:sqref>G66:G93 G102:G104 G106:G108 G100 G129:G470</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{30C25733-E64C-466F-9988-EBA8C30F2241}">
           <x14:formula1>
-            <xm:f>codebook!$C$71:$C$81</xm:f>
+            <xm:f>codebook!$C$72:$C$82</xm:f>
           </x14:formula1>
-          <xm:sqref>W66:W74 W130:W471 W77:W93 W102:W108 W98</xm:sqref>
+          <xm:sqref>W66:W74 W98 W102:W108 W77:W93 W130:W471</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1404BC5-4FF5-4C04-B486-DE592A3F3DB4}">
           <x14:formula1>
@@ -18398,13 +18483,13 @@
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK160:AK439</xm:sqref>
+          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK160:AK162 AK165:AK439</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD855EAF-C81E-44C4-996E-D61F7541B9CE}">
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\arkiv\2021-06-08\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AK156:AK159 AL150:AL437</xm:sqref>
+          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AK156:AK159 AL150:AL437 AK163:AK164</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -21865,27 +21950,27 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8AC3997-9850-4D0F-BE39-23883909EC25}">
           <x14:formula1>
-            <xm:f>codebook!$C$88:$C$122</xm:f>
+            <xm:f>codebook!$C$89:$C$123</xm:f>
           </x14:formula1>
-          <xm:sqref>B100 C360:C626 B231:B248 B112:B219 B22 B76 B279:B626</xm:sqref>
+          <xm:sqref>B100 B279:B626 B76 B22 B112:B219 B231:B248 C360:C626</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FA48F9AD-477C-41FE-97D8-9AD05DED636F}">
           <x14:formula1>
-            <xm:f>codebook!$C$134:$C$135</xm:f>
+            <xm:f>codebook!$C$135:$C$136</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F173 F175:F219 F231:F248 F278:F460 F258 F261 F263 F267:F273</xm:sqref>
+          <xm:sqref>F2:F173 F267:F273 F263 F261 F258 F278:F460 F231:F248 F175:F219</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2460B3D9-2072-4464-9488-612B96EFB2E9}">
           <x14:formula1>
-            <xm:f>codebook!$C$125:$C$130</xm:f>
+            <xm:f>codebook!$C$126:$C$131</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C219 C231:C248 C278:C359</xm:sqref>
+          <xm:sqref>C2:C219 C278:C359 C231:C248</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{04A790D0-A615-4B6C-9BDC-FC8B8EE8C3AC}">
           <x14:formula1>
-            <xm:f>codebook!$C$176:$C$178</xm:f>
+            <xm:f>codebook!$C$177:$C$179</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E219 E231:E248 E278:E626</xm:sqref>
+          <xm:sqref>E2:E219 E278:E626 E231:E248</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B43BAAAC-1456-4172-9CF9-606CEA860D5F}">
           <x14:formula1>
@@ -22756,15 +22841,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2C06C4C4-7BE4-4595-B3FF-1B88F7AE9525}">
           <x14:formula1>
-            <xm:f>codebook!$C$148:$C$175</xm:f>
+            <xm:f>codebook!$C$149:$C$176</xm:f>
           </x14:formula1>
-          <xm:sqref>C24:C45 C47:C54 C62:C631</xm:sqref>
+          <xm:sqref>C24:C45 C62:C631 C47:C54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BDAAE0E-9072-48C3-A217-6517A70E8E8C}">
           <x14:formula1>
-            <xm:f>codebook!$C$136:$C$147</xm:f>
+            <xm:f>codebook!$C$137:$C$148</xm:f>
           </x14:formula1>
-          <xm:sqref>B24:B45 B47:B54 B62:B631</xm:sqref>
+          <xm:sqref>B24:B45 B62:B631 B47:B54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5407EE94-21A5-4331-A79D-6AFA5E8047EC}">
           <x14:formula1>
@@ -24612,10 +24697,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D57AF8F-1D16-4411-BBD5-963EC5A9A56B}">
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24842,1279 +24927,1287 @@
         <v>19</v>
       </c>
       <c r="C26" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30">
         <v>3</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>15</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>0</v>
       </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>67</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>0</v>
       </c>
-      <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>1</v>
-      </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>99</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>1</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>208</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>709</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>408</v>
+        <v>709</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>443</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46">
         <v>99</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>24</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>1</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>216</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>672</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>1190</v>
+        <v>672</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58">
         <v>99</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>16</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>0</v>
       </c>
-      <c r="C58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59">
-        <v>1</v>
-      </c>
       <c r="C59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>17</v>
-      </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61">
-        <v>2</v>
-      </c>
-      <c r="C61" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>277</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>702</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>1271</v>
+        <v>702</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69">
         <v>99</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>462</v>
       </c>
-      <c r="B69">
+      <c r="B70">
         <v>0</v>
       </c>
-      <c r="C69" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70">
-        <v>1</v>
-      </c>
       <c r="C70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>10</v>
-      </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72">
-        <v>2</v>
-      </c>
-      <c r="C72" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>469</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>107</v>
+        <v>469</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>658</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>635</v>
+        <v>658</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>918</v>
+        <v>635</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>1035</v>
+        <v>918</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B81">
+        <v>10</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82">
         <v>11</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>11</v>
       </c>
-      <c r="B82">
+      <c r="B83">
         <v>1</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83">
-        <v>2</v>
-      </c>
-      <c r="C83" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85">
         <v>3</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>19</v>
       </c>
-      <c r="B85">
+      <c r="B86">
         <v>1</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86">
-        <v>2</v>
-      </c>
-      <c r="C86" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88">
         <v>3</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>68</v>
       </c>
-      <c r="B88">
+      <c r="B89">
         <v>1</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89">
-        <v>2</v>
-      </c>
-      <c r="C89" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>69</v>
+        <v>475</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>1157</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>578</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>72</v>
+        <v>578</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>377</v>
+        <v>73</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>75</v>
+        <v>377</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C99" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C101" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C102" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C103" t="s">
-        <v>376</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
-        <v>17</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="C104" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>369</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>81</v>
+        <v>369</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>447</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>390</v>
+        <v>447</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>87</v>
+        <v>390</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>370</v>
+        <v>91</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>92</v>
+        <v>371</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>1156</v>
+        <v>92</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>375</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B124">
+        <v>36</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B125">
         <v>37</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C125" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>729</v>
       </c>
-      <c r="B125">
+      <c r="B126">
         <v>0</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C126" s="3" t="s">
         <v>730</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B126">
-        <v>1</v>
-      </c>
-      <c r="C126" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>3</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>731</v>
+        <v>2</v>
+      </c>
+      <c r="C128" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B129">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B130">
+        <v>4</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B131">
         <v>5</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C131" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B131">
+      <c r="B132">
         <v>1</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>364</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132">
-        <v>2</v>
-      </c>
-      <c r="C132" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B134">
         <v>3</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>593</v>
       </c>
-      <c r="B134">
+      <c r="B135">
         <v>1</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C135" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B135">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B136">
         <v>2</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>411</v>
       </c>
-      <c r="B136">
+      <c r="B137">
         <v>1</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>412</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137">
-        <v>2</v>
-      </c>
-      <c r="C137" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>582</v>
+        <v>413</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>417</v>
+        <v>582</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C145" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>695</v>
+        <v>415</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B147">
+        <v>11</v>
+      </c>
+      <c r="C147" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B148">
         <v>12</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C148" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>343</v>
       </c>
-      <c r="B148">
+      <c r="B149">
         <v>1</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>344</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B149">
-        <v>2</v>
-      </c>
-      <c r="C149" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C150" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C151" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B152">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>380</v>
+        <v>348</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>349</v>
+        <v>420</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C155" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B157">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C157" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C158" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C159" t="s">
-        <v>421</v>
+        <v>351</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B160">
+        <v>12</v>
+      </c>
+      <c r="C160" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161">
         <v>13</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C161" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B161">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162">
         <v>14</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C162" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B162">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163">
         <v>15</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C163" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B163">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164">
         <v>16</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C164" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165">
         <v>17</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C165" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B165">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166">
         <v>18</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C166" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B166">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B167">
         <v>19</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C167" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B167">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168">
         <v>20</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C168" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B168">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B169">
         <v>21</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C169" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B169">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170">
         <v>22</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B170">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B171">
         <v>23</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C171" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B171">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B172">
         <v>24</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C172" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B172">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173">
         <v>25</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C173" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B173">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174">
         <v>26</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B174">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B175">
         <v>27</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C175" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B175">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176">
         <v>28</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>401</v>
       </c>
-      <c r="B176">
+      <c r="B177">
         <v>1</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C177" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B178">
         <v>2</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C178" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B179">
         <v>99</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C179" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ACWR and categorization metrics
</commit_message>
<xml_diff>
--- a/tl_injury_studies.xlsx
+++ b/tl_injury_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Prosjekter\Bache-Mathiesen-Biostatistikk\Data\tl_injury_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC17C44-2FEF-42A4-BD77-6BF1F287C514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8090185-D3B2-4FDB-A011-CCB030CE391C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{600D6FDA-F450-421F-B930-2043329111D1}"/>
   </bookViews>
   <sheets>
     <sheet name="study_characteristics" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4481" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4507" uniqueCount="1301">
   <si>
     <t>study_id</t>
   </si>
@@ -4019,6 +4019,21 @@
   </si>
   <si>
     <t>Analysis of the injuries and workload evolution using the RPE and s-RPE method in basketball</t>
+  </si>
+  <si>
+    <t>Many variants were copared</t>
+  </si>
+  <si>
+    <t>Principal components</t>
+  </si>
+  <si>
+    <t>Sioud</t>
+  </si>
+  <si>
+    <t>Effects of Game Weekly Frequency on Subjective Training Load, Wellness, and Injury Rate in Male Elite Soccer Players</t>
+  </si>
+  <si>
+    <t>Relationships between training load, peak height velocity, muscle soreness and fatigue status in elite-level young soccer players: a competition season study</t>
   </si>
 </sst>
 </file>
@@ -4584,13 +4599,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F660AD0-3EF8-4CB0-98FE-08F04F705623}">
-  <dimension ref="A1:AU164"/>
+  <dimension ref="A1:AU166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AD145" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AD131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD155" sqref="AD155"/>
+      <selection pane="bottomRight" activeCell="AN161" sqref="AN161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15098,6 +15113,9 @@
       <c r="AE108" t="s">
         <v>49</v>
       </c>
+      <c r="AF108" t="s">
+        <v>48</v>
+      </c>
       <c r="AK108" t="s">
         <v>48</v>
       </c>
@@ -16089,6 +16107,9 @@
       <c r="AA120" t="s">
         <v>1145</v>
       </c>
+      <c r="AF120" t="s">
+        <v>48</v>
+      </c>
       <c r="AK120" t="s">
         <v>49</v>
       </c>
@@ -16106,6 +16127,9 @@
       </c>
       <c r="AR120" t="s">
         <v>48</v>
+      </c>
+      <c r="AT120" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="121" spans="1:47" x14ac:dyDescent="0.25">
@@ -16163,8 +16187,14 @@
       <c r="X121" t="s">
         <v>1146</v>
       </c>
+      <c r="Z121" t="s">
+        <v>51</v>
+      </c>
       <c r="AA121" t="s">
         <v>1147</v>
+      </c>
+      <c r="AF121" t="s">
+        <v>49</v>
       </c>
       <c r="AK121" t="s">
         <v>48</v>
@@ -16231,6 +16261,12 @@
       <c r="Y122" t="s">
         <v>109</v>
       </c>
+      <c r="Z122" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF122" t="s">
+        <v>49</v>
+      </c>
       <c r="AK122" t="s">
         <v>48</v>
       </c>
@@ -16314,6 +16350,9 @@
       <c r="AE123" t="s">
         <v>49</v>
       </c>
+      <c r="AF123" t="s">
+        <v>49</v>
+      </c>
       <c r="AK123" t="s">
         <v>49</v>
       </c>
@@ -16397,6 +16436,9 @@
       <c r="AA124" t="s">
         <v>1149</v>
       </c>
+      <c r="AF124" t="s">
+        <v>48</v>
+      </c>
       <c r="AK124" t="s">
         <v>48</v>
       </c>
@@ -17665,7 +17707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>147</v>
       </c>
@@ -17700,7 +17742,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="146" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>148</v>
       </c>
@@ -17735,7 +17777,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>149</v>
       </c>
@@ -17773,7 +17815,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>150</v>
       </c>
@@ -17805,7 +17847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="149" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>151</v>
       </c>
@@ -17846,7 +17888,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>152</v>
       </c>
@@ -17884,7 +17926,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="151" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>153</v>
       </c>
@@ -17916,7 +17958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>154</v>
       </c>
@@ -17957,7 +17999,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="153" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>155</v>
       </c>
@@ -17973,11 +18015,35 @@
       <c r="G153" t="s">
         <v>37</v>
       </c>
+      <c r="H153">
+        <v>12</v>
+      </c>
+      <c r="I153">
+        <v>12</v>
+      </c>
       <c r="Z153" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="154" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AA153" t="s">
+        <v>1296</v>
+      </c>
+      <c r="AF153" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK153" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL153" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN153">
+        <v>18.7</v>
+      </c>
+      <c r="AP153">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>157</v>
       </c>
@@ -18009,7 +18075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>158</v>
       </c>
@@ -18050,7 +18116,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>159</v>
       </c>
@@ -18088,7 +18154,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>160</v>
       </c>
@@ -18126,7 +18192,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="158" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>161</v>
       </c>
@@ -18170,7 +18236,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="159" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>162</v>
       </c>
@@ -18196,7 +18262,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>163</v>
       </c>
@@ -18243,7 +18309,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="161" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>164</v>
       </c>
@@ -18266,7 +18332,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="162" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>165</v>
       </c>
@@ -18289,7 +18355,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="163" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>166</v>
       </c>
@@ -18321,7 +18387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="164" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>167</v>
       </c>
@@ -18356,6 +18422,73 @@
         <v>48</v>
       </c>
       <c r="AK164" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="165" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>168</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C165">
+        <v>2022</v>
+      </c>
+      <c r="D165" t="s">
+        <v>1299</v>
+      </c>
+      <c r="G165" t="s">
+        <v>32</v>
+      </c>
+      <c r="H165">
+        <v>14</v>
+      </c>
+      <c r="I165">
+        <v>14</v>
+      </c>
+      <c r="Z165" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF165" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK165" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR165" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="166" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>169</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C166">
+        <v>2023</v>
+      </c>
+      <c r="D166" t="s">
+        <v>1300</v>
+      </c>
+      <c r="G166" t="s">
+        <v>32</v>
+      </c>
+      <c r="H166">
+        <v>20</v>
+      </c>
+      <c r="I166">
+        <v>20</v>
+      </c>
+      <c r="Z166" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF166" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK166" t="s">
         <v>48</v>
       </c>
     </row>
@@ -18483,13 +18616,13 @@
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AE109:AG126 AE105:AG105 AE101:AG101 Y109:Z126 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 AK153 AK155 AK160:AK162 AK165:AK439</xm:sqref>
+          <xm:sqref>AK100:AK126 L48:L93 U79:V79 U62:V62 K119 W112:W116 T112:T116 T109:T110 W109:W110 AB109:AB126 AB105 AB101 E109:G126 E105:G105 E101:G101 AR109:AR126 AR105 AR101 AK48:AK93 AK153 AE105:AG105 AE101:AG101 AK167:AK439 Y105:Z105 Y101:Z101 T117:W126 T111:W111 T105:V105 T101:W101 L100:L126 W129 L129 AK131 L131:L132 AK133:AK134 AK137:AK138 AK142 AK145:AK146 AK149:AK150 L134:L439 Y109:Z126 AK155 AK160:AK162 AE109:AG126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD855EAF-C81E-44C4-996E-D61F7541B9CE}">
           <x14:formula1>
             <xm:f>'O:\Prosjekter\Bache-Mathiesen-002-missing-data\Data\arkiv\2021-06-08\[studies_missing_reporting.xlsx]codebook'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AK156:AK159 AL150:AL437 AK163:AK164</xm:sqref>
+          <xm:sqref>AL47:AL94 AL100:AL130 T133 AR127:AR128 AB127:AB128 AE127:AG128 AK127:AK130 AK132 Y127:Z128 W127:W128 T127:T128 T131 L127:L128 L130 E127:G128 L133 AK139:AK141 AL132:AL133 AK135:AL136 AK143:AK144 AK147:AK148 AL139:AL148 AK151:AK152 AK154 AK156:AK159 AK163:AK166 AL150:AL437</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>